<commit_message>
Addressed typos and formatting
Addressed typos and formatting
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-Coverage.xlsx
+++ b/output/carin-rtpbc-Coverage.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="397">
   <si>
     <t>Path</t>
   </si>
@@ -913,9 +913,6 @@
     <t>Pharmacy coverage identifiers</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t xml:space="preserve">BackboneElement
 </t>
   </si>
@@ -931,9 +928,6 @@
   <si>
     <t xml:space="preserve">value:type}
 </t>
-  </si>
-  <si>
-    <t>closed</t>
   </si>
   <si>
     <t>Coverage.class.id</t>
@@ -1050,7 +1044,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>group-id</t>
+    <t>rxgroup-id</t>
   </si>
   <si>
     <t>Pharmacy Benefit Group ID</t>
@@ -1062,7 +1056,7 @@
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
     &lt;system value="http://terminology.hl7.org/CodeSystem/coverage-class"/&gt;
-    &lt;code value="group"/&gt;
+    &lt;code value="rxgroup"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
@@ -5612,7 +5606,7 @@
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>289</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>52</v>
@@ -5624,19 +5618,19 @@
         <v>42</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K36" t="s" s="2">
         <v>288</v>
       </c>
       <c r="L36" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="M36" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="N36" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>42</v>
@@ -5673,16 +5667,16 @@
         <v>42</v>
       </c>
       <c r="AA36" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB36" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC36" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AD36" t="s" s="2">
-        <v>295</v>
+        <v>211</v>
       </c>
       <c r="AE36" t="s" s="2">
         <v>287</v>
@@ -5720,7 +5714,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5835,7 +5829,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5952,11 +5946,11 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5978,10 +5972,10 @@
         <v>97</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M39" t="s" s="2">
         <v>100</v>
@@ -6036,7 +6030,7 @@
         <v>42</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6071,7 +6065,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6097,14 +6091,14 @@
         <v>132</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>42</v>
@@ -6132,10 +6126,10 @@
         <v>179</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>42</v>
@@ -6153,7 +6147,7 @@
         <v>42</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>51</v>
@@ -6188,7 +6182,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6214,16 +6208,16 @@
         <v>53</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>42</v>
@@ -6272,7 +6266,7 @@
         <v>42</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>51</v>
@@ -6296,18 +6290,18 @@
         <v>42</v>
       </c>
       <c r="AM41" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN41" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO41" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO41" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6333,14 +6327,14 @@
         <v>53</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>42</v>
@@ -6389,7 +6383,7 @@
         <v>42</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6413,13 +6407,13 @@
         <v>42</v>
       </c>
       <c r="AM42" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN42" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO42" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN42" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO42" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="43">
@@ -6427,13 +6421,13 @@
         <v>287</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C43" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E43" t="s" s="2">
         <v>43</v>
@@ -6451,19 +6445,19 @@
         <v>42</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="L43" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>324</v>
-      </c>
       <c r="N43" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>42</v>
@@ -6547,7 +6541,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6662,7 +6656,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6779,11 +6773,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6805,10 +6799,10 @@
         <v>97</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>100</v>
@@ -6863,7 +6857,7 @@
         <v>42</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6898,7 +6892,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6924,14 +6918,14 @@
         <v>132</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>42</v>
@@ -6941,7 +6935,7 @@
         <v>42</v>
       </c>
       <c r="R47" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="S47" t="s" s="2">
         <v>42</v>
@@ -6959,10 +6953,10 @@
         <v>179</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>42</v>
@@ -6980,7 +6974,7 @@
         <v>42</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>51</v>
@@ -7015,7 +7009,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7041,16 +7035,16 @@
         <v>53</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>42</v>
@@ -7099,7 +7093,7 @@
         <v>42</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>51</v>
@@ -7123,18 +7117,18 @@
         <v>42</v>
       </c>
       <c r="AM48" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7160,14 +7154,14 @@
         <v>53</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>42</v>
@@ -7216,7 +7210,7 @@
         <v>42</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7240,13 +7234,13 @@
         <v>42</v>
       </c>
       <c r="AM49" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO49" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="50">
@@ -7254,13 +7248,13 @@
         <v>287</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C50" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D50" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E50" t="s" s="2">
         <v>43</v>
@@ -7278,19 +7272,19 @@
         <v>42</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>42</v>
@@ -7374,7 +7368,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7489,7 +7483,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7606,11 +7600,11 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
@@ -7632,10 +7626,10 @@
         <v>97</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M53" t="s" s="2">
         <v>100</v>
@@ -7690,7 +7684,7 @@
         <v>42</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7725,7 +7719,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7751,14 +7745,14 @@
         <v>132</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>42</v>
@@ -7768,7 +7762,7 @@
         <v>42</v>
       </c>
       <c r="R54" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S54" t="s" s="2">
         <v>42</v>
@@ -7786,10 +7780,10 @@
         <v>179</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>42</v>
@@ -7807,7 +7801,7 @@
         <v>42</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>51</v>
@@ -7842,7 +7836,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7868,16 +7862,16 @@
         <v>53</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>42</v>
@@ -7926,7 +7920,7 @@
         <v>42</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>51</v>
@@ -7950,18 +7944,18 @@
         <v>42</v>
       </c>
       <c r="AM55" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO55" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN55" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO55" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7987,14 +7981,14 @@
         <v>53</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>42</v>
@@ -8043,7 +8037,7 @@
         <v>42</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8067,13 +8061,13 @@
         <v>42</v>
       </c>
       <c r="AM56" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO56" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN56" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO56" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="57">
@@ -8081,13 +8075,13 @@
         <v>287</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C57" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D57" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E57" t="s" s="2">
         <v>43</v>
@@ -8105,19 +8099,19 @@
         <v>42</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>42</v>
@@ -8201,7 +8195,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8316,7 +8310,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8433,11 +8427,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8459,10 +8453,10 @@
         <v>97</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>100</v>
@@ -8517,7 +8511,7 @@
         <v>42</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8552,7 +8546,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8578,14 +8572,14 @@
         <v>132</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>42</v>
@@ -8595,7 +8589,7 @@
         <v>42</v>
       </c>
       <c r="R61" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S61" t="s" s="2">
         <v>42</v>
@@ -8613,10 +8607,10 @@
         <v>179</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>42</v>
@@ -8634,7 +8628,7 @@
         <v>42</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>51</v>
@@ -8669,7 +8663,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8695,16 +8689,16 @@
         <v>53</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M62" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="N62" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>42</v>
@@ -8753,7 +8747,7 @@
         <v>42</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>51</v>
@@ -8777,18 +8771,18 @@
         <v>42</v>
       </c>
       <c r="AM62" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN62" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO62" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO62" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8814,14 +8808,14 @@
         <v>53</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>42</v>
@@ -8870,7 +8864,7 @@
         <v>42</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -8894,13 +8888,13 @@
         <v>42</v>
       </c>
       <c r="AM63" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN63" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO63" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO63" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="64">
@@ -8908,13 +8902,13 @@
         <v>287</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C64" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D64" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E64" t="s" s="2">
         <v>43</v>
@@ -8932,19 +8926,19 @@
         <v>42</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>42</v>
@@ -9028,7 +9022,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9143,7 +9137,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9260,11 +9254,11 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
@@ -9286,10 +9280,10 @@
         <v>97</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M67" t="s" s="2">
         <v>100</v>
@@ -9344,7 +9338,7 @@
         <v>42</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9379,7 +9373,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9405,14 +9399,14 @@
         <v>132</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>42</v>
@@ -9422,7 +9416,7 @@
         <v>42</v>
       </c>
       <c r="R68" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="S68" t="s" s="2">
         <v>42</v>
@@ -9440,10 +9434,10 @@
         <v>179</v>
       </c>
       <c r="X68" t="s" s="2">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Z68" t="s" s="2">
         <v>42</v>
@@ -9461,7 +9455,7 @@
         <v>42</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>51</v>
@@ -9496,7 +9490,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9522,16 +9516,16 @@
         <v>53</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M69" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="L69" t="s" s="2">
+      <c r="N69" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>42</v>
@@ -9580,7 +9574,7 @@
         <v>42</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>51</v>
@@ -9604,18 +9598,18 @@
         <v>42</v>
       </c>
       <c r="AM69" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN69" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO69" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN69" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO69" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9641,14 +9635,14 @@
         <v>53</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>42</v>
@@ -9697,7 +9691,7 @@
         <v>42</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>43</v>
@@ -9721,18 +9715,18 @@
         <v>42</v>
       </c>
       <c r="AM70" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN70" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO70" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO70" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9755,17 +9749,17 @@
         <v>52</v>
       </c>
       <c r="J71" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="K71" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="K71" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>341</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>42</v>
@@ -9814,7 +9808,7 @@
         <v>42</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>43</v>
@@ -9849,7 +9843,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9875,14 +9869,14 @@
         <v>53</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O72" t="s" s="2">
         <v>42</v>
@@ -9931,7 +9925,7 @@
         <v>42</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>43</v>
@@ -9955,7 +9949,7 @@
         <v>42</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>42</v>
@@ -9966,11 +9960,11 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
@@ -9989,19 +9983,19 @@
         <v>42</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="L73" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="L73" t="s" s="2">
+      <c r="N73" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>353</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>42</v>
@@ -10050,7 +10044,7 @@
         <v>42</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>43</v>
@@ -10085,7 +10079,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10200,7 +10194,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10317,11 +10311,11 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
@@ -10343,10 +10337,10 @@
         <v>97</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M76" t="s" s="2">
         <v>100</v>
@@ -10401,7 +10395,7 @@
         <v>42</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>43</v>
@@ -10436,7 +10430,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10462,16 +10456,16 @@
         <v>132</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L77" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="M77" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="N77" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>42</v>
@@ -10499,10 +10493,10 @@
         <v>179</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="Z77" t="s" s="2">
         <v>42</v>
@@ -10520,7 +10514,7 @@
         <v>42</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>43</v>
@@ -10555,7 +10549,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -10578,19 +10572,19 @@
         <v>52</v>
       </c>
       <c r="J78" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="K78" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="K78" t="s" s="2">
+      <c r="M78" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="L78" t="s" s="2">
+      <c r="N78" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="O78" t="s" s="2">
         <v>42</v>
@@ -10639,7 +10633,7 @@
         <v>42</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>51</v>
@@ -10663,18 +10657,18 @@
         <v>42</v>
       </c>
       <c r="AM78" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="AN78" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="AO78" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="AN78" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="AO78" t="s" s="2">
-        <v>316</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10697,17 +10691,17 @@
         <v>42</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>42</v>
@@ -10756,7 +10750,7 @@
         <v>42</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>43</v>
@@ -10791,7 +10785,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10906,7 +10900,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -11023,11 +11017,11 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -11049,10 +11043,10 @@
         <v>97</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="M82" t="s" s="2">
         <v>100</v>
@@ -11107,7 +11101,7 @@
         <v>42</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>43</v>
@@ -11142,7 +11136,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -11168,14 +11162,14 @@
         <v>132</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>42</v>
@@ -11200,14 +11194,14 @@
         <v>42</v>
       </c>
       <c r="W83" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="X83" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="Y83" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="X83" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="Y83" t="s" s="2">
-        <v>382</v>
-      </c>
       <c r="Z83" t="s" s="2">
         <v>42</v>
       </c>
@@ -11224,7 +11218,7 @@
         <v>42</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>51</v>
@@ -11259,7 +11253,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11285,14 +11279,14 @@
         <v>184</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="O84" t="s" s="2">
         <v>42</v>
@@ -11341,7 +11335,7 @@
         <v>42</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>43</v>
@@ -11376,7 +11370,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11399,19 +11393,19 @@
         <v>42</v>
       </c>
       <c r="J85" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="K85" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="L85" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="K85" t="s" s="2">
+      <c r="M85" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="L85" t="s" s="2">
+      <c r="N85" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="N85" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="O85" t="s" s="2">
         <v>42</v>
@@ -11460,7 +11454,7 @@
         <v>42</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>43</v>
@@ -11495,7 +11489,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -11518,17 +11512,17 @@
         <v>42</v>
       </c>
       <c r="J86" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="K86" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L86" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="K86" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="L86" t="s" s="2">
-        <v>396</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>42</v>
@@ -11577,7 +11571,7 @@
         <v>42</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>43</v>
@@ -11604,7 +11598,7 @@
         <v>147</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>149</v>

</xml_diff>